<commit_message>
added few more programs for evaluation and minor bug fixes
</commit_message>
<xml_diff>
--- a/evaluate/outice.xlsx
+++ b/evaluate/outice.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -926,17 +926,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>p02909</t>
+          <t>p02879</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>s502766942.cob</t>
+          <t>s055491155.cob</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>s502766942.py</t>
+          <t>s055491155.py</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -944,24 +944,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>23/23</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>p02909</t>
+          <t>p02879</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>s880642132.cob</t>
+          <t>s914345468.cob</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>s880642132.py</t>
+          <t>s914345468.py</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -969,24 +969,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>23/23</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>p02915</t>
+          <t>p02909</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>s250806848.cob</t>
+          <t>s502766942.cob</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>s250806848.py</t>
+          <t>s502766942.py</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -994,24 +994,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>3/3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>p02993</t>
+          <t>p02909</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>s111459231.cob</t>
+          <t>s880642132.cob</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>s111459231.py</t>
+          <t>s880642132.py</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1019,24 +1019,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>3/3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>p03029</t>
+          <t>p02915</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>s018605057.cob</t>
+          <t>s250806848.cob</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>s018605057.py</t>
+          <t>s250806848.py</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1044,24 +1044,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>p03085</t>
+          <t>p02993</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>s247348869.cob</t>
+          <t>s111459231.cob</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>s247348869.py</t>
+          <t>s111459231.py</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1069,24 +1069,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>p03085</t>
+          <t>p03029</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>s794500343.cob</t>
+          <t>s018605057.cob</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>s794500343.py</t>
+          <t>s018605057.py</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1094,24 +1094,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>p03101</t>
+          <t>p03085</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>s563515874.cob</t>
+          <t>s247348869.cob</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>s563515874.py</t>
+          <t>s247348869.py</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1119,24 +1119,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>15/15</t>
+          <t>4/4</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>p03238</t>
+          <t>p03085</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>s739597451.cob</t>
+          <t>s794500343.cob</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>s739597451.py</t>
+          <t>s794500343.py</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1144,24 +1144,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>7/7</t>
+          <t>4/4</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>p03260</t>
+          <t>p03101</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>s346414249.cob</t>
+          <t>s563515874.cob</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>s346414249.py</t>
+          <t>s563515874.py</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1169,24 +1169,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>15/15</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>p03315</t>
+          <t>p03238</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>s910259082.cob</t>
+          <t>s739597451.cob</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>s910259082.py</t>
+          <t>s739597451.py</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1194,24 +1194,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>8/8</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>p03316</t>
+          <t>p03260</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>s513397080.cob</t>
+          <t>s346414249.cob</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>s513397080.py</t>
+          <t>s346414249.py</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1219,32 +1219,382 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>p03315</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>s910259082.cob</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>s910259082.py</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>100</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>8/8</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>p03316</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>s513397080.cob</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>s513397080.py</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>100</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>11/11</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>p03331</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>s251999208.cob</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>s251999208.py</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>50</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>p03415</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>s342220458.cob</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>s342220458.py</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>100</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>p03415</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>s760213038.cob</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>s760213038.py</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>p03433</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>s378680164.cob</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>s378680164.py</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>100</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>p03433</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>s910105267.cob</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>s910105267.py</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>100</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>p03493</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>s535106378.cob</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>s535106378.py</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>100</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>p03605</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>s655098455.cob</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>s655098455.py</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>100</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>90/90</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>p03605</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>s724623140.cob</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>s724623140.py</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>100</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>90/90</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>p03623</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>s498016040.cob</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>s498016040.py</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>100</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>p03693</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>s862197544.cob</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>s862197544.py</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>p03737</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>s496684777.cob</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>s496684777.py</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>100</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>p03795</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>s725157986.cob</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>s725157986.py</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>100</v>
-      </c>
-      <c r="E33" t="inlineStr">
+      <c r="D46" t="n">
+        <v>100</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>p03544</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>s498531048.cob</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>s498531048.py</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0/13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added more cobol files for evaluation
</commit_message>
<xml_diff>
--- a/evaluate/outice.xlsx
+++ b/evaluate/outice.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -651,17 +651,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>p02699</t>
+          <t>p02687</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>s639613950.cob</t>
+          <t>s244469283.cob</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>s639613950.py</t>
+          <t>s244469283.py</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -669,24 +669,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>p02699</t>
+          <t>p02687</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>s914372407.cob</t>
+          <t>s289948831.cob</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>s914372407.py</t>
+          <t>s289948831.py</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -694,24 +694,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>p02729</t>
+          <t>p02693</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>s421082227.cob</t>
+          <t>s344890597.cob</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>s421082227.py</t>
+          <t>s344890597.py</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -719,24 +719,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>p02766</t>
+          <t>p02693</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>s324477316.cob</t>
+          <t>s636149329.cob</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>s324477316.py</t>
+          <t>s636149329.py</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -744,24 +744,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>10/10</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>p02771</t>
+          <t>p02699</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>s228737535.cob</t>
+          <t>s639613950.cob</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>s228737535.py</t>
+          <t>s639613950.py</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -769,24 +769,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>p02771</t>
+          <t>p02699</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>s322012796.cob</t>
+          <t>s914372407.cob</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>s322012796.py</t>
+          <t>s914372407.py</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -794,24 +794,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>p02771</t>
+          <t>p02700</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>s872644229.cob</t>
+          <t>s337122046.cob</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>s872644229.py</t>
+          <t>s337122046.py</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -826,17 +826,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>p02777</t>
+          <t>p02700</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>s609549297.cob</t>
+          <t>s673976272.cob</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>s609549297.py</t>
+          <t>s673976272.py</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -844,49 +844,49 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>p02777</t>
+          <t>p02700</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>s632261802.cob</t>
+          <t>s718384914.cob</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>s632261802.py</t>
+          <t>s718384914.py</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>45.45454545454545</v>
+        <v>100</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5/11</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>p02817</t>
+          <t>p02729</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>s182051352.cob</t>
+          <t>s421082227.cob</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>s182051352.py</t>
+          <t>s421082227.py</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -894,24 +894,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6/6</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>p02847</t>
+          <t>p02766</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>s604061226.cob</t>
+          <t>s324477316.cob</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>s604061226.py</t>
+          <t>s324477316.py</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -919,24 +919,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>7/7</t>
+          <t>10/10</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>p02879</t>
+          <t>p02771</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>s055491155.cob</t>
+          <t>s228737535.cob</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>s055491155.py</t>
+          <t>s228737535.py</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -944,24 +944,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>23/23</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>p02879</t>
+          <t>p02771</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>s914345468.cob</t>
+          <t>s322012796.cob</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>s914345468.py</t>
+          <t>s322012796.py</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -969,24 +969,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>23/23</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>p02909</t>
+          <t>p02771</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>s502766942.cob</t>
+          <t>s872644229.cob</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>s502766942.py</t>
+          <t>s872644229.py</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -994,24 +994,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>p02909</t>
+          <t>p02777</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>s880642132.cob</t>
+          <t>s609549297.cob</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>s880642132.py</t>
+          <t>s609549297.py</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1019,49 +1019,49 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>p02915</t>
+          <t>p02777</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>s250806848.cob</t>
+          <t>s632261802.cob</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>s250806848.py</t>
+          <t>s632261802.py</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>100</v>
+        <v>45.45454545454545</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>5/11</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>p02993</t>
+          <t>p02789</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>s111459231.cob</t>
+          <t>s625349106.cob</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>s111459231.py</t>
+          <t>s625349106.py</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1076,17 +1076,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>p03029</t>
+          <t>p02789</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>s018605057.cob</t>
+          <t>s651301451.cob</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>s018605057.py</t>
+          <t>s651301451.py</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1094,24 +1094,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>p03085</t>
+          <t>p02789</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>s247348869.cob</t>
+          <t>s963730394.cob</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>s247348869.py</t>
+          <t>s963730394.py</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1119,24 +1119,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>p03085</t>
+          <t>p02817</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>s794500343.cob</t>
+          <t>s182051352.cob</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>s794500343.py</t>
+          <t>s182051352.py</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1144,24 +1144,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>6/6</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>p03101</t>
+          <t>p02829</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>s563515874.cob</t>
+          <t>s484078761.cob</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>s563515874.py</t>
+          <t>s484078761.py</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1169,24 +1169,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>15/15</t>
+          <t>6/6</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>p03238</t>
+          <t>p02835</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>s739597451.cob</t>
+          <t>s530754787.cob</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>s739597451.py</t>
+          <t>s530754787.py</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1194,24 +1194,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>7/7</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>p03260</t>
+          <t>p02847</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>s346414249.cob</t>
+          <t>s604061226.cob</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>s346414249.py</t>
+          <t>s604061226.py</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1219,24 +1219,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>p03315</t>
+          <t>p02879</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>s910259082.cob</t>
+          <t>s055491155.cob</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>s910259082.py</t>
+          <t>s055491155.py</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1244,24 +1244,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>8/8</t>
+          <t>23/23</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>p03316</t>
+          <t>p02879</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>s513397080.cob</t>
+          <t>s914345468.cob</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>s513397080.py</t>
+          <t>s914345468.py</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1269,49 +1269,49 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>23/23</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>p03331</t>
+          <t>p02909</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>s251999208.cob</t>
+          <t>s502766942.cob</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>s251999208.py</t>
+          <t>s502766942.py</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1/2</t>
+          <t>3/3</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>p03415</t>
+          <t>p02909</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>s342220458.cob</t>
+          <t>s880642132.cob</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>s342220458.py</t>
+          <t>s880642132.py</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1319,24 +1319,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>3/3</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>p03415</t>
+          <t>p02915</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>s760213038.cob</t>
+          <t>s250806848.cob</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>s760213038.py</t>
+          <t>s250806848.py</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1344,24 +1344,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>p03433</t>
+          <t>p02993</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>s378680164.cob</t>
+          <t>s111459231.cob</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>s378680164.py</t>
+          <t>s111459231.py</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1369,24 +1369,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>p03433</t>
+          <t>p03029</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>s910105267.cob</t>
+          <t>s018605057.cob</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>s910105267.py</t>
+          <t>s018605057.py</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1394,24 +1394,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>p03493</t>
+          <t>p03085</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>s535106378.cob</t>
+          <t>s247348869.cob</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>s535106378.py</t>
+          <t>s247348869.py</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1419,24 +1419,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>4/4</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>p03605</t>
+          <t>p03085</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>s655098455.cob</t>
+          <t>s794500343.cob</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>s655098455.py</t>
+          <t>s794500343.py</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1444,24 +1444,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>90/90</t>
+          <t>4/4</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>p03605</t>
+          <t>p03101</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>s724623140.cob</t>
+          <t>s563515874.cob</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>s724623140.py</t>
+          <t>s563515874.py</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>90/90</t>
+          <t>15/15</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>p03623</t>
+          <t>p03238</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>s498016040.cob</t>
+          <t>s739597451.cob</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>s498016040.py</t>
+          <t>s739597451.py</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1494,49 +1494,49 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>p03693</t>
+          <t>p03260</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>s862197544.cob</t>
+          <t>s346414249.cob</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>s862197544.py</t>
+          <t>s346414249.py</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0/2</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>p03737</t>
+          <t>p03288</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>s496684777.cob</t>
+          <t>s228929734.cob</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>s496684777.py</t>
+          <t>s228929734.py</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1544,24 +1544,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>p03795</t>
+          <t>p03315</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>s725157986.cob</t>
+          <t>s910259082.cob</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>s725157986.py</t>
+          <t>s910259082.py</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1569,32 +1569,732 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>8/8</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>p03544</t>
+          <t>p03316</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>s498531048.cob</t>
+          <t>s513397080.cob</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>s498531048.py</t>
+          <t>s513397080.py</t>
         </is>
       </c>
       <c r="D47" t="n">
+        <v>100</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>11/11</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>p03323</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>s070261901.cob</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>s070261901.py</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>100</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>10/10</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>p03327</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>s060305458.cob</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>s060305458.py</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>100</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>9/9</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>p03327</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>s212808048.cob</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>s212808048.py</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>100</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>9/9</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>p03331</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>s251999208.cob</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>s251999208.py</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>50</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>p03415</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>s342220458.cob</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>s342220458.py</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>100</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>p03415</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>s760213038.cob</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>s760213038.py</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>100</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>p03433</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>s378680164.cob</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>s378680164.py</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>100</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>p03433</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>s910105267.cob</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>s910105267.py</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>100</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>p03493</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>s535106378.cob</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>s535106378.py</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>100</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>s085833664.cob</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>s085833664.py</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>100</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>s150692985.cob</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>s150692985.py</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>100</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>s218625712.cob</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>s218625712.py</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>100</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>s697781232.cob</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>s697781232.py</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>100</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>s982822262.cob</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>s982822262.py</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>100</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>p03547</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>s707971310.cob</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>s707971310.py</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>p03605</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>s655098455.cob</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>s655098455.py</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>100</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>90/90</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>p03605</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>s724623140.cob</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>s724623140.py</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>100</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>90/90</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>p03623</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>s498016040.cob</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>s498016040.py</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>100</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>p03679</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>s440675024.cob</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>s440675024.py</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>100</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>p03693</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>s862197544.cob</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>s862197544.py</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
         <v>0</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>0/13</t>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>p03737</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>s496684777.cob</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>s496684777.py</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>100</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>p03777</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>s562875340.cob</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>s562875340.py</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>100</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>p03777</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>s685973551.cob</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>s685973551.py</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>100</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>p03795</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>s725157986.cob</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>s725157986.py</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>100</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>p03943</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>s127402962.cob</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>s127402962.py</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>100</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>p03962</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>s442498794.cob</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>s442498794.py</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>100</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>p03962</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>s593903284.cob</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>s593903284.py</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>100</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>p03962</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>s686116970.cob</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>s686116970.py</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>100</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2/2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added few  more cobol files for evaluation
</commit_message>
<xml_diff>
--- a/evaluate/outice.xlsx
+++ b/evaluate/outice.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>p02594</t>
+          <t>p02552</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>s303983970.cob</t>
+          <t>s252298897.cob</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>s303983970.py</t>
+          <t>s252298897.py</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -469,24 +469,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>10/10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>p02612</t>
+          <t>p02594</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>s019381271.cob</t>
+          <t>s303983970.cob</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>s019381271.py</t>
+          <t>s303983970.py</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -494,7 +494,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>17/17</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
@@ -506,12 +506,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>s274424021.cob</t>
+          <t>s019381271.cob</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>s274424021.py</t>
+          <t>s019381271.py</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -526,17 +526,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>p02627</t>
+          <t>p02612</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>s799013402.cob</t>
+          <t>s274424021.cob</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>s799013402.py</t>
+          <t>s274424021.py</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -544,7 +544,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10/10</t>
+          <t>17/17</t>
         </is>
       </c>
     </row>
@@ -556,12 +556,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>s903521318.cob</t>
+          <t>s799013402.cob</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>s903521318.py</t>
+          <t>s799013402.py</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -576,100 +576,100 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>p02640</t>
+          <t>p02627</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>s348198913.cob</t>
+          <t>s903521318.cob</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>s348198913.py</t>
+          <t>s903521318.py</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>86.66666666666667</v>
+        <v>100</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>13/15</t>
+          <t>10/10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>p02663</t>
+          <t>p02640</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>s581403666.cob</t>
+          <t>s348198913.cob</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>s581403666.py</t>
+          <t>s348198913.py</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>100</v>
+        <v>86.66666666666667</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>13/15</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>p02682</t>
+          <t>p02663</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>s918496651.cob</t>
+          <t>s581403666.cob</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>s918496651.py</t>
+          <t>s581403666.py</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>93.33333333333333</v>
+        <v>100</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>14/15</t>
+          <t>2/2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>p02687</t>
+          <t>p02682</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>s244469283.cob</t>
+          <t>s918496651.cob</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>s244469283.py</t>
+          <t>s918496651.py</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>100</v>
+        <v>93.33333333333333</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>7/7</t>
+          <t>14/15</t>
         </is>
       </c>
     </row>
@@ -681,12 +681,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>s289948831.cob</t>
+          <t>s244469283.cob</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>s289948831.py</t>
+          <t>s244469283.py</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -701,17 +701,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>p02693</t>
+          <t>p02687</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>s344890597.cob</t>
+          <t>s289948831.cob</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>s344890597.py</t>
+          <t>s289948831.py</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -719,7 +719,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
@@ -731,12 +731,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>s636149329.cob</t>
+          <t>s344890597.cob</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>s636149329.py</t>
+          <t>s344890597.py</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -751,17 +751,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>p02699</t>
+          <t>p02693</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>s639613950.cob</t>
+          <t>s636149329.cob</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>s639613950.py</t>
+          <t>s636149329.py</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -781,12 +781,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>s914372407.cob</t>
+          <t>s639613950.cob</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>s914372407.py</t>
+          <t>s639613950.py</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -801,17 +801,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>p02700</t>
+          <t>p02699</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>s337122046.cob</t>
+          <t>s914372407.cob</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>s337122046.py</t>
+          <t>s914372407.py</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -819,7 +819,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
@@ -831,12 +831,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>s673976272.cob</t>
+          <t>s337122046.cob</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>s673976272.py</t>
+          <t>s337122046.py</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -856,12 +856,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>s718384914.cob</t>
+          <t>s673976272.cob</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>s718384914.py</t>
+          <t>s673976272.py</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -876,17 +876,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>p02729</t>
+          <t>p02700</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>s421082227.cob</t>
+          <t>s718384914.cob</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>s421082227.py</t>
+          <t>s718384914.py</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -901,17 +901,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>p02766</t>
+          <t>p02729</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>s324477316.cob</t>
+          <t>s421082227.cob</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>s324477316.py</t>
+          <t>s421082227.py</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -919,24 +919,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>10/10</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>p02771</t>
+          <t>p02753</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>s228737535.cob</t>
+          <t>s138398313.cob</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>s228737535.py</t>
+          <t>s138398313.py</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -944,24 +944,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>p02771</t>
+          <t>p02753</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>s322012796.cob</t>
+          <t>s358090291.cob</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>s322012796.py</t>
+          <t>s358090291.py</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -969,24 +969,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>p02771</t>
+          <t>p02766</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>s872644229.cob</t>
+          <t>s324477316.cob</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>s872644229.py</t>
+          <t>s324477316.py</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -994,24 +994,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>10/10</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>p02777</t>
+          <t>p02771</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>s609549297.cob</t>
+          <t>s228737535.cob</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>s609549297.py</t>
+          <t>s228737535.py</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1019,49 +1019,49 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>p02777</t>
+          <t>p02771</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>s632261802.cob</t>
+          <t>s322012796.cob</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>s632261802.py</t>
+          <t>s322012796.py</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>45.45454545454545</v>
+        <v>100</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>5/11</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>p02789</t>
+          <t>p02771</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>s625349106.cob</t>
+          <t>s872644229.cob</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>s625349106.py</t>
+          <t>s872644229.py</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1069,24 +1069,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>p02789</t>
+          <t>p02777</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>s651301451.cob</t>
+          <t>s609549297.cob</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>s651301451.py</t>
+          <t>s609549297.py</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1094,49 +1094,49 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>p02789</t>
+          <t>p02777</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>s963730394.cob</t>
+          <t>s632261802.cob</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>s963730394.py</t>
+          <t>s632261802.py</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>100</v>
+        <v>45.45454545454545</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>5/11</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>p02817</t>
+          <t>p02789</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>s182051352.cob</t>
+          <t>s625349106.cob</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>s182051352.py</t>
+          <t>s625349106.py</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1144,24 +1144,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>6/6</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>p02829</t>
+          <t>p02789</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>s484078761.cob</t>
+          <t>s651301451.cob</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>s484078761.py</t>
+          <t>s651301451.py</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1169,24 +1169,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>6/6</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>p02835</t>
+          <t>p02789</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>s530754787.cob</t>
+          <t>s963730394.cob</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>s530754787.py</t>
+          <t>s963730394.py</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1194,24 +1194,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>12/12</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>p02847</t>
+          <t>p02811</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>s604061226.cob</t>
+          <t>s140105459.cob</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>s604061226.py</t>
+          <t>s140105459.py</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1226,17 +1226,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>p02879</t>
+          <t>p02811</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>s055491155.cob</t>
+          <t>s533487001.cob</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>s055491155.py</t>
+          <t>s533487001.py</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1244,24 +1244,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>23/23</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>p02879</t>
+          <t>p02811</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>s914345468.cob</t>
+          <t>s823275518.cob</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>s914345468.py</t>
+          <t>s823275518.py</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1269,24 +1269,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>23/23</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>p02909</t>
+          <t>p02811</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>s502766942.cob</t>
+          <t>s971400288.cob</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>s502766942.py</t>
+          <t>s971400288.py</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1294,24 +1294,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>p02909</t>
+          <t>p02817</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>s880642132.cob</t>
+          <t>s182051352.cob</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>s880642132.py</t>
+          <t>s182051352.py</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1319,24 +1319,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>6/6</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>p02915</t>
+          <t>p02829</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>s250806848.cob</t>
+          <t>s484078761.cob</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>s250806848.py</t>
+          <t>s484078761.py</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1344,24 +1344,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>6/6</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>p02993</t>
+          <t>p02835</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>s111459231.cob</t>
+          <t>s530754787.cob</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>s111459231.py</t>
+          <t>s530754787.py</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1369,24 +1369,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>13/13</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>p03029</t>
+          <t>p02847</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>s018605057.cob</t>
+          <t>s604061226.cob</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>s018605057.py</t>
+          <t>s604061226.py</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1394,24 +1394,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>p03085</t>
+          <t>p02879</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>s247348869.cob</t>
+          <t>s055491155.cob</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>s247348869.py</t>
+          <t>s055491155.py</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1419,24 +1419,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>23/23</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>p03085</t>
+          <t>p02879</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>s794500343.cob</t>
+          <t>s914345468.cob</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>s794500343.py</t>
+          <t>s914345468.py</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1444,24 +1444,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>23/23</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>p03101</t>
+          <t>p02909</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>s563515874.cob</t>
+          <t>s502766942.cob</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>s563515874.py</t>
+          <t>s502766942.py</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>15/15</t>
+          <t>3/3</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>p03238</t>
+          <t>p02909</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>s739597451.cob</t>
+          <t>s880642132.cob</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>s739597451.py</t>
+          <t>s880642132.py</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1494,24 +1494,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>7/7</t>
+          <t>3/3</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>p03260</t>
+          <t>p02915</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>s346414249.cob</t>
+          <t>s250806848.cob</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>s346414249.py</t>
+          <t>s250806848.py</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1526,17 +1526,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>p03288</t>
+          <t>p02933</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>s228929734.cob</t>
+          <t>s246223241.cob</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>s228929734.py</t>
+          <t>s246223241.py</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1551,17 +1551,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>p03315</t>
+          <t>p02933</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>s910259082.cob</t>
+          <t>s333645860.cob</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>s910259082.py</t>
+          <t>s333645860.py</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1569,24 +1569,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>8/8</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>p03316</t>
+          <t>p02969</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>s513397080.cob</t>
+          <t>s648537227.cob</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>s513397080.py</t>
+          <t>s648537227.py</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1594,24 +1594,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>11/11</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>p03323</t>
+          <t>p02969</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>s070261901.cob</t>
+          <t>s708854140.cob</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>s070261901.py</t>
+          <t>s708854140.py</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1619,24 +1619,24 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>10/10</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>p03327</t>
+          <t>p02987</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>s060305458.cob</t>
+          <t>s717698035.cob</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>s060305458.py</t>
+          <t>s717698035.py</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1644,24 +1644,24 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>p03327</t>
+          <t>p02993</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>s212808048.cob</t>
+          <t>s111459231.cob</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>s212808048.py</t>
+          <t>s111459231.py</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1669,49 +1669,49 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>p03331</t>
+          <t>p02999</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>s251999208.cob</t>
+          <t>s077344104.cob</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>s251999208.py</t>
+          <t>s077344104.py</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1/2</t>
+          <t>13/13</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>p03415</t>
+          <t>p03029</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>s342220458.cob</t>
+          <t>s018605057.cob</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>s342220458.py</t>
+          <t>s018605057.py</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1719,24 +1719,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>p03415</t>
+          <t>p03075</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>s760213038.cob</t>
+          <t>s071690090.cob</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>s760213038.py</t>
+          <t>s071690090.py</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1744,24 +1744,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>p03433</t>
+          <t>p03075</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>s378680164.cob</t>
+          <t>s959412799.cob</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>s378680164.py</t>
+          <t>s959412799.py</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1769,24 +1769,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>p03433</t>
+          <t>p03085</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>s910105267.cob</t>
+          <t>s247348869.cob</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>s910105267.py</t>
+          <t>s247348869.py</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1794,24 +1794,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>4/4</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>p03493</t>
+          <t>p03085</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>s535106378.cob</t>
+          <t>s794500343.cob</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>s535106378.py</t>
+          <t>s794500343.py</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1819,24 +1819,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>4/4</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>p03543</t>
+          <t>p03101</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>s085833664.cob</t>
+          <t>s563515874.cob</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>s085833664.py</t>
+          <t>s563515874.py</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1844,24 +1844,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>15/15</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>p03543</t>
+          <t>p03206</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>s150692985.cob</t>
+          <t>s274524816.cob</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>s150692985.py</t>
+          <t>s274524816.py</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1876,17 +1876,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>p03543</t>
+          <t>p03206</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>s218625712.cob</t>
+          <t>s318123532.cob</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>s218625712.py</t>
+          <t>s318123532.py</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1901,17 +1901,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>p03543</t>
+          <t>p03210</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>s697781232.cob</t>
+          <t>s807120571.cob</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>s697781232.py</t>
+          <t>s807120571.py</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1919,24 +1919,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>p03543</t>
+          <t>p03238</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>s982822262.cob</t>
+          <t>s739597451.cob</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>s982822262.py</t>
+          <t>s739597451.py</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1944,24 +1944,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>7/7</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>p03547</t>
+          <t>p03243</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>s707971310.cob</t>
+          <t>s232998445.cob</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>s707971310.py</t>
+          <t>s232998445.py</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1969,24 +1969,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>p03605</t>
+          <t>p03260</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>s655098455.cob</t>
+          <t>s346414249.cob</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>s655098455.py</t>
+          <t>s346414249.py</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1994,24 +1994,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>90/90</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>p03605</t>
+          <t>p03284</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>s724623140.cob</t>
+          <t>s038241548.cob</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>s724623140.py</t>
+          <t>s038241548.py</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2019,24 +2019,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>90/90</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>p03623</t>
+          <t>p03284</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>s498016040.cob</t>
+          <t>s457297332.cob</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>s498016040.py</t>
+          <t>s457297332.py</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2044,24 +2044,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>12/12</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>p03679</t>
+          <t>p03288</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>s440675024.cob</t>
+          <t>s228929734.cob</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>s440675024.py</t>
+          <t>s228929734.py</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2069,49 +2069,49 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>p03693</t>
+          <t>p03315</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>s862197544.cob</t>
+          <t>s910259082.cob</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>s862197544.py</t>
+          <t>s910259082.py</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>0/2</t>
+          <t>8/8</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>p03737</t>
+          <t>p03316</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>s496684777.cob</t>
+          <t>s513397080.cob</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>s496684777.py</t>
+          <t>s513397080.py</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2119,24 +2119,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>11/11</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>p03777</t>
+          <t>p03323</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>s562875340.cob</t>
+          <t>s070261901.cob</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>s562875340.py</t>
+          <t>s070261901.py</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>10/10</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>p03777</t>
+          <t>p03327</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>s685973551.cob</t>
+          <t>s060305458.cob</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>s685973551.py</t>
+          <t>s060305458.py</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2169,24 +2169,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>p03795</t>
+          <t>p03327</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>s725157986.cob</t>
+          <t>s212808048.cob</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>s725157986.py</t>
+          <t>s212808048.py</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2194,49 +2194,49 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>9/9</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>p03943</t>
+          <t>p03331</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>s127402962.cob</t>
+          <t>s251999208.cob</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>s127402962.py</t>
+          <t>s251999208.py</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>1/2</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>p03962</t>
+          <t>p03351</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>s442498794.cob</t>
+          <t>s599184617.cob</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>s442498794.py</t>
+          <t>s599184617.py</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -2244,24 +2244,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>50/50</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>p03962</t>
+          <t>p03415</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>s593903284.cob</t>
+          <t>s342220458.cob</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>s593903284.py</t>
+          <t>s342220458.py</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2276,23 +2276,748 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>p03415</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>s760213038.cob</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>s760213038.py</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>100</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>p03433</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>s378680164.cob</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>s378680164.py</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>100</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>p03433</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>s910105267.cob</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>s910105267.py</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>100</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>p03493</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>s535106378.cob</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>s535106378.py</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>100</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>s085833664.cob</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>s085833664.py</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>100</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>s150692985.cob</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>s150692985.py</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>100</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>s218625712.cob</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>s218625712.py</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>100</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>s697781232.cob</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>s697781232.py</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>100</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>p03543</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>s982822262.cob</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>s982822262.py</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>100</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>p03547</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>s707971310.cob</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>s707971310.py</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>100</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>p03605</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>s655098455.cob</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>s655098455.py</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>100</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>90/90</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>p03605</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>s724623140.cob</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>s724623140.py</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>100</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>90/90</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>p03623</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>s498016040.cob</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>s498016040.py</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>100</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>p03679</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>s440675024.cob</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>s440675024.py</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>100</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>p03719</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>s681020301.cob</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>s681020301.py</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>100</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>p03737</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>s496684777.cob</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>s496684777.py</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>100</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>p03759</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>s408741745.cob</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>s408741745.py</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>100</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>p03759</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>s782907931.cob</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>s782907931.py</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>100</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>p03777</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>s562875340.cob</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>s562875340.py</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>100</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>p03777</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>s685973551.cob</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>s685973551.py</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>100</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>p03795</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>s725157986.cob</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>s725157986.py</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>100</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>p03813</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>s102841374.cob</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>s102841374.py</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>100</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>p03834</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>s332782304.cob</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>s332782304.py</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>100</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>10/10</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>p03943</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>s127402962.cob</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>s127402962.py</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>100</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
           <t>p03962</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>s442498794.cob</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>s442498794.py</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>100</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>p03962</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>s593903284.cob</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>s593903284.py</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>100</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>p03962</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
         <is>
           <t>s686116970.cob</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>s686116970.py</t>
         </is>
       </c>
-      <c r="D75" t="n">
-        <v>100</v>
-      </c>
-      <c r="E75" t="inlineStr">
+      <c r="D101" t="n">
+        <v>100</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>p04043</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>s691919214.cob</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>s691919214.py</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>100</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>p04043</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>s694891543.cob</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>s694891543.py</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>100</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>p04043</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>s713437627.cob</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>s713437627.py</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>100</v>
+      </c>
+      <c r="E104" t="inlineStr">
         <is>
           <t>2/2</t>
         </is>

</xml_diff>